<commit_message>
feat: Implement comprehensive candidate job management module including listing, creation, status updates, and Excel import/export.
</commit_message>
<xml_diff>
--- a/public/sample_excel/jobs-example.xlsx
+++ b/public/sample_excel/jobs-example.xlsx
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37696,6 +37696,23 @@
       <c r="AY1000" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"MALE,FEMALE,OTHER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
+      <formula1>"HINDU,MUSLIM,CHRISTIAN,SIKH,BUDDHIST,JAIN,OTHER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576">
+      <formula1>"FACE TO FACE,ONLINE,DIRECT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG1048576">
+      <formula1>"FIT,UNFIT,REPEAT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
+      <formula1>"ECR,ECNR"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>